<commit_message>
Updated Banquet & Gene
</commit_message>
<xml_diff>
--- a/src/data/All_Inductees.xlsx
+++ b/src/data/All_Inductees.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nevascared-m1/jrhof-website-app/jrhof-web-app/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nevascared-m1/GitHub Cloned/jrhof-webapp/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95026525-C0F4-854A-A627-84E5DA24AB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99775CCE-59D2-DB42-A324-2C76B85C09E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="6500" windowWidth="16960" windowHeight="22300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,15 +224,6 @@
     <t>James_Roorda</t>
   </si>
   <si>
-    <t>Gene Rozzelle</t>
-  </si>
-  <si>
-    <t>Gene_Rozzelle.jpg</t>
-  </si>
-  <si>
-    <t>Gene_Rozzelle</t>
-  </si>
-  <si>
     <t>Sal Salazar</t>
   </si>
   <si>
@@ -1377,6 +1368,15 @@
   </si>
   <si>
     <t>Myran_Dunker</t>
+  </si>
+  <si>
+    <t>Gene Rozelle</t>
+  </si>
+  <si>
+    <t>Gene_Rozelle.jpg</t>
+  </si>
+  <si>
+    <t>Gene_Rozelle</t>
   </si>
 </sst>
 </file>
@@ -1739,8 +1739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1779,7 +1779,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1908,7 +1908,7 @@
         <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1925,7 +1925,7 @@
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1942,7 +1942,7 @@
         <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -2001,7 +2001,7 @@
         <v>52</v>
       </c>
       <c r="E17" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -2048,1860 +2048,1860 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>444</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>445</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>446</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E27" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B31" s="2">
         <v>1987</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E31" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B32" s="2">
         <v>1989</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B33" s="2">
         <v>1990</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B34" s="2">
         <v>1990</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B35" s="2">
         <v>1990</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B36" s="2">
         <v>1990</v>
       </c>
       <c r="C36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B37" s="2">
         <v>1990</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B38" s="2">
         <v>1990</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D38" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E38" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B39" s="2">
         <v>1990</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B40" s="2">
         <v>1990</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B41" s="2">
         <v>1990</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B42" s="2">
         <v>1991</v>
       </c>
       <c r="C42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D42" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B43" s="2">
         <v>1991</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E43" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B44" s="2">
         <v>1991</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D44" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B45" s="2">
         <v>1991</v>
       </c>
       <c r="C45" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B46" s="2">
         <v>1992</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D46" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E46" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B47" s="2">
         <v>1992</v>
       </c>
       <c r="C47" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B48" s="2">
         <v>1992</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D48" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B49" s="2">
         <v>1992</v>
       </c>
       <c r="C49" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D49" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E49" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B50" s="2">
         <v>1992</v>
       </c>
       <c r="C50" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D50" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B51" s="2">
         <v>1992</v>
       </c>
       <c r="C51" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D51" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B52" s="2">
         <v>1993</v>
       </c>
       <c r="C52" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D52" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B53" s="2">
         <v>1993</v>
       </c>
       <c r="C53" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D53" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B54" s="2">
         <v>1993</v>
       </c>
       <c r="C54" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D54" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E54" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B55" s="2">
         <v>1993</v>
       </c>
       <c r="C55" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E55" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B56" s="2">
         <v>1994</v>
       </c>
       <c r="C56" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D56" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E56" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B57" s="2">
         <v>1994</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D57" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E57" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B58" s="2">
         <v>1994</v>
       </c>
       <c r="C58" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B59" s="2">
         <v>1994</v>
       </c>
       <c r="C59" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D59" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B60" s="2">
         <v>1995</v>
       </c>
       <c r="C60" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D60" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E60" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B61" s="2">
         <v>1995</v>
       </c>
       <c r="C61" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D61" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E61" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B62" s="2">
         <v>1995</v>
       </c>
       <c r="C62" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D62" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E62" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B63" s="2">
         <v>1996</v>
       </c>
       <c r="C63" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D63" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B64" s="2">
         <v>1996</v>
       </c>
       <c r="C64" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D64" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B65" s="2">
         <v>2007</v>
       </c>
       <c r="C65" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D65" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B66" s="2">
         <v>1996</v>
       </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B67" s="2">
         <v>1996</v>
       </c>
       <c r="C67" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D67" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B68" s="2">
         <v>1997</v>
       </c>
       <c r="C68" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D68" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B69" s="2">
         <v>1997</v>
       </c>
       <c r="C69" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D69" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B70" s="2">
         <v>1997</v>
       </c>
       <c r="C70" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D70" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B71" s="2">
         <v>1997</v>
       </c>
       <c r="C71" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D71" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B72" s="2">
         <v>1998</v>
       </c>
       <c r="C72" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D72" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B73" s="2">
         <v>1998</v>
       </c>
       <c r="C73" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D73" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B74" s="2">
         <v>1999</v>
       </c>
       <c r="C74" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D74" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B75" s="2">
         <v>1999</v>
       </c>
       <c r="C75" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D75" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B76" s="2">
         <v>1999</v>
       </c>
       <c r="C76" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D76" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B77" s="2">
         <v>2000</v>
       </c>
       <c r="C77" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D77" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B78" s="2">
         <v>2000</v>
       </c>
       <c r="C78" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D78" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B79" s="2">
         <v>2000</v>
       </c>
       <c r="C79" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D79" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B80" s="2">
         <v>2000</v>
       </c>
       <c r="C80" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D80" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E80" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B81" s="2">
         <v>2001</v>
       </c>
       <c r="C81" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D81" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B82" s="2">
         <v>2001</v>
       </c>
       <c r="C82" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D82" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B83" s="2">
         <v>2002</v>
       </c>
       <c r="C83" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D83" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B84" s="2">
         <v>2002</v>
       </c>
       <c r="C84" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D84" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B85" s="2">
         <v>2002</v>
       </c>
       <c r="C85" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D85" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B86" s="2">
         <v>2002</v>
       </c>
       <c r="C86" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D86" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B87" s="2">
         <v>2002</v>
       </c>
       <c r="C87" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D87" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B88" s="2">
         <v>2003</v>
       </c>
       <c r="C88" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D88" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B89" s="2">
         <v>2003</v>
       </c>
       <c r="C89" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D89" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B90" s="2">
         <v>2004</v>
       </c>
       <c r="C90" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D90" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B91" s="2">
         <v>2004</v>
       </c>
       <c r="C91" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D91" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B92" s="2">
         <v>2004</v>
       </c>
       <c r="C92" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D92" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B93" s="2">
         <v>2005</v>
       </c>
       <c r="C93" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D93" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B94" s="2">
         <v>2006</v>
       </c>
       <c r="C94" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D94" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B95" s="2">
         <v>2006</v>
       </c>
       <c r="C95" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D95" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B96" s="2">
         <v>2006</v>
       </c>
       <c r="C96" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D96" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B97" s="2">
         <v>2006</v>
       </c>
       <c r="C97" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D97" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B98" s="2">
         <v>2007</v>
       </c>
       <c r="C98" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D98" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B99" s="2">
         <v>2008</v>
       </c>
       <c r="C99" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D99" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B100" s="2">
         <v>2008</v>
       </c>
       <c r="C100" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D100" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B101" s="2">
         <v>2008</v>
       </c>
       <c r="C101" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D101" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B102" s="2">
         <v>2008</v>
       </c>
       <c r="C102" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D102" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B103" s="2">
         <v>2008</v>
       </c>
       <c r="C103" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D103" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B104" s="2">
         <v>2009</v>
       </c>
       <c r="C104" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D104" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B105" s="2">
         <v>2009</v>
       </c>
       <c r="C105" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D105" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B106" s="2">
         <v>2009</v>
       </c>
       <c r="C106" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D106" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B107" s="2">
         <v>2009</v>
       </c>
       <c r="C107" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D107" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B108" s="2">
         <v>2010</v>
       </c>
       <c r="C108" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D108" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B109" s="2">
         <v>2010</v>
       </c>
       <c r="C109" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D109" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B110" s="2">
         <v>2010</v>
       </c>
       <c r="C110" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D110" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B111" s="2">
         <v>2011</v>
       </c>
       <c r="C111" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D111" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B112" s="2">
         <v>2011</v>
       </c>
       <c r="C112" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D112" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B113" s="2">
         <v>2011</v>
       </c>
       <c r="C113" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D113" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B114" s="2">
         <v>2012</v>
       </c>
       <c r="C114" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D114" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B115" s="2">
         <v>2012</v>
       </c>
       <c r="C115" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D115" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B116" s="2">
         <v>2012</v>
       </c>
       <c r="C116" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D116" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B117" s="2">
         <v>2013</v>
       </c>
       <c r="C117" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D117" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B118" s="2">
         <v>2013</v>
       </c>
       <c r="C118" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D118" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B119" s="2">
         <v>2013</v>
       </c>
       <c r="C119" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D119" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B120" s="2">
         <v>2014</v>
       </c>
       <c r="C120" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D120" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B121" s="2">
         <v>2014</v>
       </c>
       <c r="C121" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D121" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B122" s="2">
         <v>2015</v>
       </c>
       <c r="C122" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D122" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B123" s="2">
         <v>2015</v>
       </c>
       <c r="C123" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D123" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B124" s="2">
         <v>2015</v>
       </c>
       <c r="C124" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D124" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B125" s="2">
         <v>2016</v>
       </c>
       <c r="C125" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D125" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B126" s="2">
         <v>2016</v>
       </c>
       <c r="C126" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D126" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B127" s="2">
         <v>2016</v>
       </c>
       <c r="C127" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D127" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B128" s="2">
         <v>2016</v>
       </c>
       <c r="C128" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D128" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B129" s="2">
         <v>2017</v>
       </c>
       <c r="C129" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D129" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B130" s="2">
         <v>2017</v>
       </c>
       <c r="C130" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D130" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B131" s="2">
         <v>2017</v>
       </c>
       <c r="C131" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D131" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B132" s="2">
         <v>2018</v>
       </c>
       <c r="C132" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D132" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B133" s="2">
         <v>2018</v>
       </c>
       <c r="C133" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D133" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B134" s="2">
         <v>2020</v>
       </c>
       <c r="C134" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D134" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E134" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B135" s="2">
         <v>2020</v>
       </c>
       <c r="C135" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D135" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E135" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B136" s="2">
         <v>2023</v>
       </c>
       <c r="C136" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D136" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B137" s="2">
         <v>2023</v>
       </c>
       <c r="C137" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D137" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B138" s="2">
         <v>2023</v>
       </c>
       <c r="C138" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D138" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B139" s="2">
         <v>2023</v>
       </c>
       <c r="C139" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D139" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B140" s="2">
         <v>1991</v>
       </c>
       <c r="C140" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D140" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D141" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E141" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B142" s="2">
         <v>2024</v>
       </c>
       <c r="C142" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D142" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B143" s="2">
         <v>2024</v>
       </c>
       <c r="C143" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D143" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B144" s="2">
         <v>2024</v>
       </c>
       <c r="C144" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D144" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="B145" s="2">
         <v>2024</v>
       </c>
       <c r="C145" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D145" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B146" s="2">
         <v>2025</v>
       </c>
       <c r="C146" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D146" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B147" s="2">
         <v>2025</v>
       </c>
       <c r="C147" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D147" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B148" s="2">
         <v>2025</v>
       </c>
       <c r="C148" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D148" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -3923,17 +3923,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="25b577db-bb44-4779-b00a-a5e86f2929e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="37757e62-f69c-4483-a9f2-10f42122d094" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BCA9808E943BA14BBD2F70AB94DD8563" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d26cae50b258b5e310e6feadd98a4fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="25b577db-bb44-4779-b00a-a5e86f2929e3" xmlns:ns3="37757e62-f69c-4483-a9f2-10f42122d094" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a4bdc8ba5d4cf608a584445e3ee47d0" ns2:_="" ns3:_="">
     <xsd:import namespace="25b577db-bb44-4779-b00a-a5e86f2929e3"/>
@@ -4134,6 +4123,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="25b577db-bb44-4779-b00a-a5e86f2929e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="37757e62-f69c-4483-a9f2-10f42122d094" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4144,17 +4144,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C52AC99-496C-4260-AD22-CBFDC8540E49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="25b577db-bb44-4779-b00a-a5e86f2929e3"/>
-    <ds:schemaRef ds:uri="37757e62-f69c-4483-a9f2-10f42122d094"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{333DCC81-0AD0-44EC-A722-3ACBA126D05F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4173,6 +4162,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C52AC99-496C-4260-AD22-CBFDC8540E49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="25b577db-bb44-4779-b00a-a5e86f2929e3"/>
+    <ds:schemaRef ds:uri="37757e62-f69c-4483-a9f2-10f42122d094"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E10FB2A6-0FC2-4268-BB00-F012139807F3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added 2026 Inductee Photos
</commit_message>
<xml_diff>
--- a/src/data/All_Inductees.xlsx
+++ b/src/data/All_Inductees.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nevascared-m1/GitHub Cloned/jrhof-webapp/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tj/jrhof-webapp/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99775CCE-59D2-DB42-A324-2C76B85C09E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D597B5E-9F9C-C644-A30F-3B551027AC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="6500" windowWidth="16960" windowHeight="22300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="3600" windowWidth="16960" windowHeight="22300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Inductees" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="456">
   <si>
     <t>Name</t>
   </si>
@@ -1377,6 +1377,33 @@
   </si>
   <si>
     <t>Gene_Rozelle</t>
+  </si>
+  <si>
+    <t>Fred Zuercher</t>
+  </si>
+  <si>
+    <t>Fred_Zuercher.jpg</t>
+  </si>
+  <si>
+    <t>Fred_Zuercher</t>
+  </si>
+  <si>
+    <t>George Demetriou</t>
+  </si>
+  <si>
+    <t>George_Demetriou.jpg</t>
+  </si>
+  <si>
+    <t>George_Demetriou</t>
+  </si>
+  <si>
+    <t>Terry Angell</t>
+  </si>
+  <si>
+    <t>Terry_Angell.jpg</t>
+  </si>
+  <si>
+    <t>Terry_Angell</t>
   </si>
 </sst>
 </file>
@@ -1739,8 +1766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3905,13 +3932,46 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B149" s="2"/>
+      <c r="A149" t="s">
+        <v>447</v>
+      </c>
+      <c r="B149" s="2">
+        <v>2026</v>
+      </c>
+      <c r="C149" t="s">
+        <v>448</v>
+      </c>
+      <c r="D149" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B150" s="2"/>
+      <c r="A150" t="s">
+        <v>450</v>
+      </c>
+      <c r="B150" s="2">
+        <v>2026</v>
+      </c>
+      <c r="C150" t="s">
+        <v>451</v>
+      </c>
+      <c r="D150" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B151" s="2"/>
+      <c r="A151" t="s">
+        <v>453</v>
+      </c>
+      <c r="B151" s="2">
+        <v>2026</v>
+      </c>
+      <c r="C151" t="s">
+        <v>454</v>
+      </c>
+      <c r="D151" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B152" s="2"/>
@@ -3923,6 +3983,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="25b577db-bb44-4779-b00a-a5e86f2929e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="37757e62-f69c-4483-a9f2-10f42122d094" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BCA9808E943BA14BBD2F70AB94DD8563" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3d26cae50b258b5e310e6feadd98a4fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="25b577db-bb44-4779-b00a-a5e86f2929e3" xmlns:ns3="37757e62-f69c-4483-a9f2-10f42122d094" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a4bdc8ba5d4cf608a584445e3ee47d0" ns2:_="" ns3:_="">
     <xsd:import namespace="25b577db-bb44-4779-b00a-a5e86f2929e3"/>
@@ -4123,17 +4194,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="25b577db-bb44-4779-b00a-a5e86f2929e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="37757e62-f69c-4483-a9f2-10f42122d094" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4144,6 +4204,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C52AC99-496C-4260-AD22-CBFDC8540E49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="25b577db-bb44-4779-b00a-a5e86f2929e3"/>
+    <ds:schemaRef ds:uri="37757e62-f69c-4483-a9f2-10f42122d094"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{333DCC81-0AD0-44EC-A722-3ACBA126D05F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4162,17 +4233,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C52AC99-496C-4260-AD22-CBFDC8540E49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="25b577db-bb44-4779-b00a-a5e86f2929e3"/>
-    <ds:schemaRef ds:uri="37757e62-f69c-4483-a9f2-10f42122d094"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E10FB2A6-0FC2-4268-BB00-F012139807F3}">
   <ds:schemaRefs>

</xml_diff>